<commit_message>
PP-3 PP-1 PP-5 #done Removed unnecessary functions and finished documentation
</commit_message>
<xml_diff>
--- a/documentation/Risk assessment.xlsx
+++ b/documentation/Risk assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dotty man K\Documents\Kester\Coding\QA-training\practical-project\LifeGoals\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DA0DA33-7C8E-4545-941B-9A0104C1C133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2ED3B0-485C-4F4D-B808-160A089D1665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B145A09D-F41C-4D83-AA76-0BA388CD40F7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Description</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>Build database back from backed up data</t>
+  </si>
+  <si>
+    <t>As there is no password or secure login, anyone who knows your username can log into your account. Should not be used to store sensitive information.</t>
+  </si>
+  <si>
+    <t>Make sure people know not to use it to store sensitive information</t>
+  </si>
+  <si>
+    <t>Take down sensitive infromation immediately and possibly inform authorities/relevant parties.</t>
+  </si>
+  <si>
+    <t>Someone getting sensitive information from your account</t>
   </si>
 </sst>
 </file>
@@ -471,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38421098-A8B2-4289-8202-259143F84CCA}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -671,6 +683,32 @@
         <v>27</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>